<commit_message>
backlog atualizado + burndown atualizado
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Grafico BurnDown.xlsx
+++ b/sprint_grupo7/TI/Grafico BurnDown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\Pesquisa e inovação\sprint_01\sprint_grupo7\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{083411A8-9F52-49CB-9193-1435C7CEF6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33A1DE7-5BE3-4375-BF61-ED92AFCC972C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3698AED0-CDD5-4485-9C23-6435B0F20BE7}"/>
+    <workbookView xWindow="1968" yWindow="24" windowWidth="21168" windowHeight="12336" activeTab="1" xr2:uid="{3698AED0-CDD5-4485-9C23-6435B0F20BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -361,16 +361,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>290</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -447,16 +447,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>290</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>272</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>186</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1647,7 +1647,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1703,10 +1703,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="E3" s="3">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="F3" s="3">
         <v>18</v>
@@ -1724,13 +1724,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
+        <v>177</v>
+      </c>
+      <c r="E4" s="3">
         <v>217</v>
       </c>
-      <c r="E4" s="3">
-        <v>272</v>
-      </c>
       <c r="F4" s="3">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1745,13 +1745,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="E5" s="3">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="F5" s="3">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1766,13 +1766,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="F6" s="3">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1"/>
     </row>

</xml_diff>